<commit_message>
git-tfs-id: [http://tfsnpt.int.thomson.com:8080/tfs/Cobalt_Collection]$/Cobalt QED Testing/PLPLusUK;C768923
</commit_message>
<xml_diff>
--- a/PPIUK-AssetPages/src/test/resources/CobaltUsers.xlsx
+++ b/PPIUK-AssetPages/src/test/resources/CobaltUsers.xlsx
@@ -1054,10 +1054,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G84"/>
+  <dimension ref="A1:G80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C80" sqref="C80"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="G84" sqref="A81:G84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2577,18 +2577,6 @@
       <c r="G80" s="10" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="81" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E81" s="9"/>
-    </row>
-    <row r="82" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E82" s="9"/>
-    </row>
-    <row r="83" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E83" s="9"/>
-    </row>
-    <row r="84" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E84" s="9"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Usman - Asset pages Optimized
git-tfs-id: [http://tfsnpt.int.thomson.com:8080/tfs/Cobalt_Collection]$/Cobalt QED Testing/PLPLusUK;C772348
</commit_message>
<xml_diff>
--- a/PPIUK-AssetPages/src/test/resources/CobaltUsers.xlsx
+++ b/PPIUK-AssetPages/src/test/resources/CobaltUsers.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="276">
   <si>
     <t>UserName</t>
   </si>
@@ -838,6 +838,12 @@
   </si>
   <si>
     <t xml:space="preserve">AssetPageUser5@mailinator.com </t>
+  </si>
+  <si>
+    <t>AssetPageUser6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AssetPageUser6@mailinator.com </t>
   </si>
 </sst>
 </file>
@@ -1258,11 +1264,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G113"/>
+  <dimension ref="A1:G114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="C63" sqref="C63"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3341,6 +3345,23 @@
       </c>
       <c r="G113" s="10" t="s">
         <v>273</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A114" s="11" t="s">
+        <v>274</v>
+      </c>
+      <c r="B114" t="s">
+        <v>52</v>
+      </c>
+      <c r="E114" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="F114" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G114" s="10" t="s">
+        <v>275</v>
       </c>
     </row>
   </sheetData>
@@ -3421,9 +3442,10 @@
     <hyperlink ref="G110" r:id="rId74"/>
     <hyperlink ref="G113" r:id="rId75"/>
     <hyperlink ref="G111" r:id="rId76" display="AssetPageUser1@mailinator.com "/>
+    <hyperlink ref="G114" r:id="rId77"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId77"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId78"/>
 </worksheet>
 </file>
 

</xml_diff>